<commit_message>
Agregando mujer numero 6
</commit_message>
<xml_diff>
--- a/CR/11_05_22BasedeDatosMDLPcorrect.xlsx
+++ b/CR/11_05_22BasedeDatosMDLPcorrect.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\Documents\PaginaWebCusco\CR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AF4BF7-F28E-4301-BB86-96F2D5206835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70285F6F-7027-4A03-B0C4-831EA2B37847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21555" yWindow="1230" windowWidth="21600" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lugar" sheetId="6" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="253">
   <si>
     <t>id</t>
   </si>
@@ -721,6 +721,165 @@
   </si>
   <si>
     <t>https://www.youtube.com/embed/v7WSLHeSR44</t>
+  </si>
+  <si>
+    <t>Antonieta</t>
+  </si>
+  <si>
+    <t>Conde Marquina</t>
+  </si>
+  <si>
+    <t>Maestra y gestora intercultural. Magíster en Educación Intercultural Bilingüe. Madre, mujer e hija del ancestral Pueblo Quechua Kʼana de Layo, Cusco. Sus áreas de interés son: Intraculturalidad e interculturalidad, investigación y gestión intercultural en temáticas socioculturales, socioeducativas, sociolingüísticas y ciudadanía intercultural vinculados a los pueblos indígenas. En su trayectoria de proyección sociocultural, académica y de vida ha realizado publicaciones, presentaciones, actividades formativas y labores profesionales, con énfasis en lo testimonial, desde el enfoque intercultural dentro y fuera del Perú. Editora y correctora independiente, en quechua y castellano, de investigaciones científico sociales, literarias e informativas (desde 2003 hasta la actualidad). Es alumni/exbecaria de la Fundación Ford, FLACSO Argentina e Ibercultura Viva, FILAC y AECID.</t>
+  </si>
+  <si>
+    <t>img/Mujer_6.jpg</t>
+  </si>
+  <si>
+    <t>antonietacondemarquina@gmail.com</t>
+  </si>
+  <si>
+    <t>-14.48242077795887</t>
+  </si>
+  <si>
+    <t>-71.15427871932138</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/aXVNtofplSk</t>
+  </si>
+  <si>
+    <t>Usos del quechua en Layo, K´ana suyupi, Cusco</t>
+  </si>
+  <si>
+    <t>Libro de investigación</t>
+  </si>
+  <si>
+    <t>Este libro explora la situación sociolingüística del uso del quechua en la comunidad de Taypitunga, Layo, Cusco. Los datos fueron recopilados a través del método etnográfico. Este método posibilitó conocer la versión directa de los hablantes, y en su propio contexto, acerca del proceso actual que el quechua presenta. Las entrevistas y las observaciones de las interacciones de uso del quechua contaron con la participación de jóvenes colegiales y por extensión a los hablantes de la comunidad en general. Los ámbitos que se tomaron como referencia fueron: el hogar, el colegio y la comunidad</t>
+  </si>
+  <si>
+    <t>img/Mujer_6_Libro1.jpg</t>
+  </si>
+  <si>
+    <t>DocPlayer</t>
+  </si>
+  <si>
+    <t>https://docplayer.es/90780283-Usos-del-quechua-en-layo-k-ana-suyupi-cusco.html</t>
+  </si>
+  <si>
+    <t>Oro hate emändoya Wachiperi : Diccionario Wachiperi Castellano / DDC-Cusco</t>
+  </si>
+  <si>
+    <t>Corrección de estilo</t>
+  </si>
+  <si>
+    <t>(Antonieta realiza la corrección de estilo) El Ministerio de Cultura presentó el Diccionario Wachiperi: Oro Hate Emändoya. La lengua wachiperi, hablada en la provincia de Paucartambo, es una variedad del harakbut. Este diccionario recoge la sabiduría, los conocimientos y expresiones propias de la cosmovisión amazónica de las comunidades nativas de Santa Rosa de Huacaria y Queros Wachiperi; y adquiere una singular importancia para los wachiperi del siglo XXI, interesados en revertir el proceso de debilitamiento en que se encuentra su pueblo ante la disminución de la práctica de su lengua.</t>
+  </si>
+  <si>
+    <t>img/Mujer_6_Libro6.jpg</t>
+  </si>
+  <si>
+    <t>Biblioteca Central DDC-Cusco</t>
+  </si>
+  <si>
+    <t>http://biblioteca.culturacusco.gob.pe/cgi-bin/koha/opac-detail.pl?biblionumber=3948</t>
+  </si>
+  <si>
+    <t>Poesía (Quechua y Castellano). Antología de Ganadores de la Categoría "C" : Premio Regional de Cultura, 2015 / Dirección Desconcentrada de Cultura Cusco</t>
+  </si>
+  <si>
+    <t>DL 201603534</t>
+  </si>
+  <si>
+    <t>(Antonieta realiza la corrección de estilo en quechua ). Antología de poemas en quechua y castellano de los ganadores de la Categoría "C". Entre los poetas de esta antología tenemos: Gladis Naty Valencia Rosell, Huchuy harawikunata; Rocío Cjuiro Mescco, Qaqarumicha. Poesía en castellano: Pável Ugarte Céspedes, Repatriación de las aves; Elvis David Quispe Altamirano, Visitame siempre en octubre; Martin Castillo Collado, Primera Dosis; Jhon Hansel Choque Condori, La Palabra no hace el amor, sino la ausencia</t>
+  </si>
+  <si>
+    <t>img/Mujer_6_Libro5.jpg</t>
+  </si>
+  <si>
+    <t>Quechua, idioma que puede hacer retornar la vida de comunidad: Runasimiqa ayllumanmi kutichinman</t>
+  </si>
+  <si>
+    <t>Ensayo</t>
+  </si>
+  <si>
+    <t>Este ensayo trata sobre la inserción tímida de este proceso reivindicativo y justiciero en el contexto y escenario histórico, simbólico, práctico, institucional, familiar, personal</t>
+  </si>
+  <si>
+    <t>img/Mujer_6_Libro2.jpg</t>
+  </si>
+  <si>
+    <t>Ariadnaediciones</t>
+  </si>
+  <si>
+    <t>https://ariadnaediciones.cl/index.php?option=com_content&amp;view=article&amp;layout=edit&amp;id=153</t>
+  </si>
+  <si>
+    <t>Poesía Súper Contemporánea de Perú y Estados Unidos.</t>
+  </si>
+  <si>
+    <t>Traducción</t>
+  </si>
+  <si>
+    <t>(Antonieta participa en el grupo de traductores de esta obra) Poesía súper contemporánea de Perú y Estados Unidos es un libro sensual y necesario. Entre sus páginas se encuentran las voces más destacadas del movimiento literario alt-lit de Estados Unidos con una intensa muestra de poesía peruana contemporánea: individual y colectiva, del campo y la ciudad, tradicional y de vanguardia al mismo tiempo.</t>
+  </si>
+  <si>
+    <t>img/Mujer_6_Libro7.jpg</t>
+  </si>
+  <si>
+    <t>Revista Saqsaywaman N°10</t>
+  </si>
+  <si>
+    <t>(Antonieta realiza la corrección de estilo en quechua ) Nuevos aportes a la Arqueología del Periodo Formativo del Cusco en Marcavalle, Minaspata y Kullupata.</t>
+  </si>
+  <si>
+    <t>img/Mujer_6_Libro4.jpg</t>
+  </si>
+  <si>
+    <t>Esta publicación no está disponible.</t>
+  </si>
+  <si>
+    <t>Balance preliminar en torno a avances, desafíos y oportunidades de la consulta previa en el Perú</t>
+  </si>
+  <si>
+    <t>El trabajo de investigación ofrece una mirada panorámica de la consulta previa en cinco apartados. Los procesos vinculados a la consulta previa vislumbran el punto de quiebre que dio origen a los diferentes eventos, etapas, acuerdos y desacuerdos que sirvieron de preámbulo a la promulgación de la ley y su reglamento.</t>
+  </si>
+  <si>
+    <t>img/Mujer_6_Libro3.jpg</t>
+  </si>
+  <si>
+    <t>Centro de Estudios Constitucionales (CEC) Colección "Derecho y Sociedad" 2017</t>
+  </si>
+  <si>
+    <t>https://www.tc.gob.pe/wp-content/uploads/2018/10/Justicia-e-interculturalidad.pdf</t>
+  </si>
+  <si>
+    <t>5to Festival Caravana de Poesía Cusco - Ayacucho</t>
+  </si>
+  <si>
+    <t>Antología de poemas en castellano y quechua.</t>
+  </si>
+  <si>
+    <t>img/Mujer_6_Libro8.jpg</t>
+  </si>
+  <si>
+    <t>Relato Puriy kutiy (El viaje del retorno)</t>
+  </si>
+  <si>
+    <t>Cuento</t>
+  </si>
+  <si>
+    <t>La autora nos comenta que este relato fue publicado en Noqanchis No. 5. revista bilingüe quechua-asháninka, 2012</t>
+  </si>
+  <si>
+    <t>img/Mujer_6_Libro9.jpg</t>
+  </si>
+  <si>
+    <t>Cr</t>
+  </si>
+  <si>
+    <t>Canas</t>
+  </si>
+  <si>
+    <t>Layo</t>
   </si>
 </sst>
 </file>
@@ -730,11 +889,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -873,8 +1039,21 @@
       <color rgb="FF4D5F72"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -935,8 +1114,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1172,259 +1357,335 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1551,7 +1812,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A1:C10" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A1:C14" headerRowDxfId="0">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="mujer_id"/>
@@ -1769,10 +2030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94D338E-FEBE-4758-8002-AA19DAC4F902}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1791,7 +2052,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="15" thickBot="1">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -1803,6 +2064,20 @@
       </c>
       <c r="D2" s="38" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1">
+      <c r="A3" s="107">
+        <v>2</v>
+      </c>
+      <c r="B3" s="108" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="108" t="s">
+        <v>251</v>
+      </c>
+      <c r="D3" s="108" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -1812,10 +2087,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1827,7 +2102,8 @@
     <col min="5" max="5" width="19.453125" customWidth="1"/>
     <col min="6" max="8" width="20.453125" customWidth="1"/>
     <col min="9" max="9" width="35.453125" customWidth="1"/>
-    <col min="10" max="11" width="16.453125" customWidth="1"/>
+    <col min="10" max="10" width="21.36328125" customWidth="1"/>
+    <col min="11" max="11" width="21.54296875" customWidth="1"/>
     <col min="12" max="12" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2047,6 +2323,42 @@
       </c>
       <c r="L6" s="87" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1" thickBot="1">
+      <c r="A7" s="88">
+        <v>6</v>
+      </c>
+      <c r="B7" s="89" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" s="89" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" s="90">
+        <v>2</v>
+      </c>
+      <c r="E7" s="91">
+        <v>29716</v>
+      </c>
+      <c r="F7" s="89"/>
+      <c r="G7" s="92" t="s">
+        <v>202</v>
+      </c>
+      <c r="H7" s="89" t="s">
+        <v>203</v>
+      </c>
+      <c r="I7" s="89" t="s">
+        <v>204</v>
+      </c>
+      <c r="J7" s="94" t="s">
+        <v>205</v>
+      </c>
+      <c r="K7" s="89" t="s">
+        <v>206</v>
+      </c>
+      <c r="L7" s="93" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2057,18 +2369,19 @@
     <hyperlink ref="L4" r:id="rId4" xr:uid="{8F48762D-C7BC-4536-9427-7E09BA386D45}"/>
     <hyperlink ref="L5" r:id="rId5" xr:uid="{00F78730-FB2C-459B-B37B-4A52A3BDAC37}"/>
     <hyperlink ref="L6" r:id="rId6" xr:uid="{97CA63DB-E1DE-4665-A6A4-5167C9B3D236}"/>
+    <hyperlink ref="L7" r:id="rId7" xr:uid="{AEC2B6C5-49C6-48EA-A4B7-29DB5B21566C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId7"/>
+  <pageSetup orientation="landscape" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2848,6 +3161,282 @@
       <c r="J25" s="71" t="s">
         <v>118</v>
       </c>
+    </row>
+    <row r="26" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A26" s="95">
+        <v>25</v>
+      </c>
+      <c r="B26" s="96" t="s">
+        <v>208</v>
+      </c>
+      <c r="C26" s="96">
+        <v>9789995415914</v>
+      </c>
+      <c r="D26" s="96" t="s">
+        <v>209</v>
+      </c>
+      <c r="E26" s="96">
+        <v>2014</v>
+      </c>
+      <c r="F26" s="96" t="s">
+        <v>210</v>
+      </c>
+      <c r="G26" s="96">
+        <v>6</v>
+      </c>
+      <c r="H26" s="96" t="s">
+        <v>211</v>
+      </c>
+      <c r="I26" s="96" t="s">
+        <v>212</v>
+      </c>
+      <c r="J26" s="61" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A27" s="97">
+        <v>26</v>
+      </c>
+      <c r="B27" s="98" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="98">
+        <v>9786124686528</v>
+      </c>
+      <c r="D27" s="98" t="s">
+        <v>215</v>
+      </c>
+      <c r="E27" s="98">
+        <v>2014</v>
+      </c>
+      <c r="F27" s="98" t="s">
+        <v>216</v>
+      </c>
+      <c r="G27" s="98">
+        <v>6</v>
+      </c>
+      <c r="H27" s="98" t="s">
+        <v>217</v>
+      </c>
+      <c r="I27" s="98" t="s">
+        <v>218</v>
+      </c>
+      <c r="J27" s="72" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A28" s="97">
+        <v>27</v>
+      </c>
+      <c r="B28" s="98" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" s="98" t="s">
+        <v>221</v>
+      </c>
+      <c r="D28" s="98" t="s">
+        <v>215</v>
+      </c>
+      <c r="E28" s="98">
+        <v>2015</v>
+      </c>
+      <c r="F28" s="98" t="s">
+        <v>222</v>
+      </c>
+      <c r="G28" s="98">
+        <v>6</v>
+      </c>
+      <c r="H28" s="98" t="s">
+        <v>223</v>
+      </c>
+      <c r="I28" s="98" t="s">
+        <v>218</v>
+      </c>
+      <c r="J28" s="100"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A29" s="97">
+        <v>28</v>
+      </c>
+      <c r="B29" s="98" t="s">
+        <v>224</v>
+      </c>
+      <c r="C29" s="98">
+        <v>9789568416461</v>
+      </c>
+      <c r="D29" s="98" t="s">
+        <v>225</v>
+      </c>
+      <c r="E29" s="98">
+        <v>2016</v>
+      </c>
+      <c r="F29" s="98" t="s">
+        <v>226</v>
+      </c>
+      <c r="G29" s="98">
+        <v>6</v>
+      </c>
+      <c r="H29" s="98" t="s">
+        <v>227</v>
+      </c>
+      <c r="I29" s="98" t="s">
+        <v>228</v>
+      </c>
+      <c r="J29" s="72" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A30" s="97">
+        <v>29</v>
+      </c>
+      <c r="B30" s="98" t="s">
+        <v>230</v>
+      </c>
+      <c r="C30" s="98">
+        <v>9789569853104</v>
+      </c>
+      <c r="D30" s="98" t="s">
+        <v>231</v>
+      </c>
+      <c r="E30" s="98">
+        <v>2017</v>
+      </c>
+      <c r="F30" s="98" t="s">
+        <v>232</v>
+      </c>
+      <c r="G30" s="98">
+        <v>6</v>
+      </c>
+      <c r="H30" s="98" t="s">
+        <v>233</v>
+      </c>
+      <c r="I30" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="J30" s="99" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A31" s="97">
+        <v>30</v>
+      </c>
+      <c r="B31" s="98" t="s">
+        <v>234</v>
+      </c>
+      <c r="C31" s="98"/>
+      <c r="D31" s="98" t="s">
+        <v>215</v>
+      </c>
+      <c r="E31" s="98">
+        <v>2018</v>
+      </c>
+      <c r="F31" s="98" t="s">
+        <v>235</v>
+      </c>
+      <c r="G31" s="98">
+        <v>6</v>
+      </c>
+      <c r="H31" s="98" t="s">
+        <v>236</v>
+      </c>
+      <c r="I31" s="98" t="s">
+        <v>237</v>
+      </c>
+      <c r="J31" s="100"/>
+    </row>
+    <row r="32" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A32" s="97">
+        <v>31</v>
+      </c>
+      <c r="B32" s="98" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32" s="98">
+        <v>9786124740831</v>
+      </c>
+      <c r="D32" s="98" t="s">
+        <v>225</v>
+      </c>
+      <c r="E32" s="98">
+        <v>2018</v>
+      </c>
+      <c r="F32" s="98" t="s">
+        <v>239</v>
+      </c>
+      <c r="G32" s="98">
+        <v>6</v>
+      </c>
+      <c r="H32" s="98" t="s">
+        <v>240</v>
+      </c>
+      <c r="I32" s="98" t="s">
+        <v>241</v>
+      </c>
+      <c r="J32" s="72" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A33" s="97">
+        <v>32</v>
+      </c>
+      <c r="B33" s="98" t="s">
+        <v>243</v>
+      </c>
+      <c r="C33" s="98">
+        <v>9786124770265</v>
+      </c>
+      <c r="D33" s="98" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="98">
+        <v>2018</v>
+      </c>
+      <c r="F33" s="98" t="s">
+        <v>244</v>
+      </c>
+      <c r="G33" s="98">
+        <v>6</v>
+      </c>
+      <c r="H33" s="98" t="s">
+        <v>245</v>
+      </c>
+      <c r="I33" s="98" t="s">
+        <v>237</v>
+      </c>
+      <c r="J33" s="101"/>
+    </row>
+    <row r="34" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A34" s="97">
+        <v>33</v>
+      </c>
+      <c r="B34" s="98" t="s">
+        <v>246</v>
+      </c>
+      <c r="C34" s="100"/>
+      <c r="D34" s="100" t="s">
+        <v>247</v>
+      </c>
+      <c r="E34" s="102">
+        <v>2012</v>
+      </c>
+      <c r="F34" s="100" t="s">
+        <v>248</v>
+      </c>
+      <c r="G34" s="98">
+        <v>6</v>
+      </c>
+      <c r="H34" s="98" t="s">
+        <v>249</v>
+      </c>
+      <c r="I34" s="98" t="s">
+        <v>237</v>
+      </c>
+      <c r="J34" s="99"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2870,10 +3459,14 @@
     <hyperlink ref="J19" r:id="rId17" xr:uid="{BF4F85EB-AEB1-440D-8960-418B5309AD83}"/>
     <hyperlink ref="J21" r:id="rId18" xr:uid="{2111296F-2B57-4012-BAEF-D71B8A9E13A2}"/>
     <hyperlink ref="J22" r:id="rId19" xr:uid="{C9574BC8-67D6-4235-A03D-F149D1D6F9A9}"/>
+    <hyperlink ref="J26" r:id="rId20" xr:uid="{8E0E9464-B85C-4B7D-90D3-F3D0C1B9E004}"/>
+    <hyperlink ref="J27" r:id="rId21" xr:uid="{C175CAED-678F-46D9-A622-39F3F731F747}"/>
+    <hyperlink ref="J29" r:id="rId22" xr:uid="{927D7676-D74D-4CA6-9B57-B4940DD53AFD}"/>
+    <hyperlink ref="J32" r:id="rId23" xr:uid="{D30080B9-7AF7-48DE-AA3E-121CC32DEA25}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId20"/>
-  <legacyDrawing r:id="rId21"/>
+  <pageSetup orientation="landscape" r:id="rId24"/>
+  <legacyDrawing r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -2882,7 +3475,7 @@
   <dimension ref="A1:C896"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2992,7 +3585,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3003,10 +3596,50 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A11" s="103">
+        <v>10</v>
+      </c>
+      <c r="B11" s="103">
+        <v>6</v>
+      </c>
+      <c r="C11" s="104" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A12" s="103">
+        <v>11</v>
+      </c>
+      <c r="B12" s="103">
+        <v>6</v>
+      </c>
+      <c r="C12" s="104" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A13" s="103">
+        <v>12</v>
+      </c>
+      <c r="B13" s="103">
+        <v>6</v>
+      </c>
+      <c r="C13" s="104" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A14" s="105">
+        <v>13</v>
+      </c>
+      <c r="B14" s="105">
+        <v>6</v>
+      </c>
+      <c r="C14" s="106" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="16" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Agregando escritora numero 6
</commit_message>
<xml_diff>
--- a/CR/11_05_22BasedeDatosMDLPcorrect.xlsx
+++ b/CR/11_05_22BasedeDatosMDLPcorrect.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\Documents\PaginaWebCusco\CR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70285F6F-7027-4A03-B0C4-831EA2B37847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1949F756-0B82-4F89-B717-FD814C46D64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21555" yWindow="1230" windowWidth="21600" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lugar" sheetId="6" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="251">
   <si>
     <t>id</t>
   </si>
@@ -143,11 +143,6 @@
   </si>
   <si>
     <t>Cule Vargas</t>
-  </si>
-  <si>
-    <t>Adriana Cule es una artista visual y retratista profesional. Se desenvuelve en el terreno del diseño gráfico, el modelado análogo y digital, el desarrollo de personajes pintorescos y la creación de cuentos cortos. En susobras busca que las perspectivas y composición interactúen con el espectador exagerando las formas.
-Ha participado en diferentes proyectos, muestras artísticas, diferentes campañas y producciones entre ellas la inauguración de Saga Falabella en Cusco, la filmación de Transformers en Cusco y la iniciativa de “Hagamos un Perú que de gusto” de Inca Kola.
-Ilustro el cuento “El zorro y el cóndor” de Maximo Ccama, realizo el libro de cuentos “Sueño Índigo”  y los cómics “Pasado” y “Colores”.</t>
   </si>
   <si>
     <t xml:space="preserve">yozoh2004@gmail.com
@@ -191,15 +186,6 @@
     <t>mujer_id</t>
   </si>
   <si>
-    <t>Sueño Indigo</t>
-  </si>
-  <si>
-    <t>9786124751028</t>
-  </si>
-  <si>
-    <t>Libro</t>
-  </si>
-  <si>
     <t>Libros que contiene dos historias tiernas, acompañadas de espectaculares ilustraciones que te transportarán junto a los protagonistas.</t>
   </si>
   <si>
@@ -230,9 +216,6 @@
     <t>Articulo de revista</t>
   </si>
   <si>
-    <t>El presente trabajo analiza la peregrinación de Sebastián “Quimichi”, a partir de la documentación que pertenece al archivo histórico del Santuario de Cocharcas, específicamente al documento denominado “Relación de la imagen de Nuestra Señora que esta en este pueblo de Cocharca hecha por el licenciado don Pedro Guillén de Mendoza en 20 de julio de 1625 años”.</t>
-  </si>
-  <si>
     <t>El archivo del Santuario de Cocharcas: historia, catalogación y transcripción paleográfica siglos XVI-XX.</t>
   </si>
   <si>
@@ -248,9 +231,6 @@
     <t>El Santuario de Cocharcas: Construcción, clero secular y participación indígena (1611-1680)</t>
   </si>
   <si>
-    <t>El presente artículo se enmarca en el difícil proceso de reorganización social y religiosa que las poblaciones indigenas padecieron dentro de la región de Huamanga en la coyuntura finissecular del siglo XVI. Nuestra preocupación por comprender dichas reorganizaciones obdece a un doble interes, primero dar cuenta de la conformacipn del espacio social de la doctrina de Chocharcas, y segundo realziar un analisis de las relaciones interétnicas y las nociones de inclusión/exclusión apartir de la implementación de la cofradía, convirtiéndose en el medio de mayor eficacia para canalizar y viabilizar los intereses colonial étnicos locales de poder para así ganarse un espacio dentro de la nueva sociedad colonial que se conformaba.</t>
-  </si>
-  <si>
     <t>Investigación histórica del Santuario de Cocharcas y el Archivo Arzobispal de Abancay.</t>
   </si>
   <si>
@@ -296,9 +276,6 @@
     <t>http://vrin.unsaac.edu.pe/publicaciones/1/vademecum-fedu-20132014.html</t>
   </si>
   <si>
-    <t>Antología Angeles y Demonios</t>
-  </si>
-  <si>
     <t>Cuentos</t>
   </si>
   <si>
@@ -308,15 +285,9 @@
     <t>Poemario</t>
   </si>
   <si>
-    <t>Éste es su primero poemario, como el título, un cúmulo de dulces y ácidas experiencias</t>
-  </si>
-  <si>
     <t>https://anamaria.pro/acidulce/</t>
   </si>
   <si>
-    <t>Mil Poemas a Cesar Vallejo: Una gesta de amor universal</t>
-  </si>
-  <si>
     <t>La hija del bosque</t>
   </si>
   <si>
@@ -479,16 +450,10 @@
     <t>Plataforma Behance</t>
   </si>
   <si>
-    <t>Antologia organziada por la Asociación Centro Cultural Cusco.</t>
-  </si>
-  <si>
     <t>Esta publicación no esta disponible.</t>
   </si>
   <si>
     <t>Sitio Web Ana María Milla</t>
-  </si>
-  <si>
-    <t>Ana María Milla participa en esta antologia con su poema en la pagina 349, esta publicación es una recopilación hecha por Alfred Asís Antología-Recopilación-Escritoras, Escritores-Poetas del Mundo.</t>
   </si>
   <si>
     <t>Enlace Drive</t>
@@ -625,9 +590,6 @@
     <t>Antología Poética del Cusco</t>
   </si>
   <si>
-    <t>Gladys Conde es acreedora de mención honrosa en poesía por el Premio Regional de Cultura de Cusco (2006), publicándose sus poesías en “Antología Poética del Cusco” realizado por el INC en el 2007.</t>
-  </si>
-  <si>
     <t>img/Mujer_4_Libro1.jpg</t>
   </si>
   <si>
@@ -669,9 +631,6 @@
     <t>http://www.casadelaliteratura.gob.pe/segundo-cancionero-del-programa-bebetecas/</t>
   </si>
   <si>
-    <t>Cuentos Aguarnas</t>
-  </si>
-  <si>
     <t>DL 2011 00716</t>
   </si>
   <si>
@@ -693,9 +652,6 @@
     <t>Artículo de revista</t>
   </si>
   <si>
-    <t>En el presente artículo la ilustradora explica: Lejos de proponer una visión romantizada de la tradición oral y la cosmovisión ancestral, pretendo brindar reflexiones desde mi práctica artística personal y desde la corriente estética del surrealismo sobre los elementos claves de la identidad y los ecosistemas en el Perú. Mucha de la influencia e inspiración nace tanto de artistas y artesanos locales como internacionales. Me enfoco en corrientes que nacieron en la colonia, como es la reconocida Escuela Cusqueña, que tiene como representantes a pintores como Diego Quispe Tito, o el pintor Italiano Bernardo Bitti. Cabe resaltar que los trabajos de la Escuela Cusqueña en mayoría son obras de pintores originarios y mestizos. Obras sacras como las del Corpus Christi siglo XVII de autor anónimo o la obra Virgen del Carmen del siglo XVII, que por su composición se asocia a la representación de la Pachamama, son importantes como antecedente de la pintura actual peruana enfocada en lo tradicional y la ecología</t>
-  </si>
-  <si>
     <t>img/Mujer_5_Libro2.jpg</t>
   </si>
   <si>
@@ -711,9 +667,6 @@
     <t>img/Mujer_5_Libro3.jpg</t>
   </si>
   <si>
-    <t>Con experiencia laboral desde el 2003 hasta la actualidad. Natalia Lizarraga ha trabajado en diferentes proyectos artísticos individuales y colectivos. Su trabajo consiste en estéticas como el surrealismo, surrealismo narrativo, que se ven reflejados en trabajos como: “Dulcinea“, “Huida a Egipto” , “Nativo“, parte del proyecto “Memoria 2014“ que constó de 4 exhibiciones realizadas en diferentes Centros Culturales del Cusco-Perú; otros trabajos con enfoque mayormente ecológico, de diferentes especies emblemáticas o en peligro de extinción a nivel nacional o internacional tenemos “Tigrillo“ 2015. Tambien en sus exposiciones se han enfocado en la cultura viva como son tradiciones orales, con obras como con la muestra realizada en la casa cultural Cusco-Perú , 2016. Otras expresiones artisticas que revalorando tradiciones y creencias mortuarios que se tienen en la actualidad que provienen desde la cosmovisión precolombina, con obras como “El condenado“, “Aparición“, “Ofrendas“ . Sobre mitos y leyendas, a nivel nacional e internacional nos deleita con obras como “El Minotauro“ 2004. Natalia Lizarraga ha tenido exposiciónes individuales y colectivas en el Perú como en el extranjero en paises como: México, Bruselas, Alemania y Estados Unidos. En el campo de la ilustración ha participando en proyecto como la publicación “Cuentos Aguarunas“ del Centro Guamán Poma de Ayala Cusco en 2010, tambien trabajo en el libro-cancionero “LLIQLLA“2021 con la Editorial SM Perú y colaborando en la portada del Álbum Musical Lliqlla de la misma cantautora Gladys Conde, Cusco, 2021.</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/embed/Nz-d6tKw4wA</t>
   </si>
   <si>
@@ -783,15 +736,9 @@
     <t>http://biblioteca.culturacusco.gob.pe/cgi-bin/koha/opac-detail.pl?biblionumber=3948</t>
   </si>
   <si>
-    <t>Poesía (Quechua y Castellano). Antología de Ganadores de la Categoría "C" : Premio Regional de Cultura, 2015 / Dirección Desconcentrada de Cultura Cusco</t>
-  </si>
-  <si>
     <t>DL 201603534</t>
   </si>
   <si>
-    <t>(Antonieta realiza la corrección de estilo en quechua ). Antología de poemas en quechua y castellano de los ganadores de la Categoría "C". Entre los poetas de esta antología tenemos: Gladis Naty Valencia Rosell, Huchuy harawikunata; Rocío Cjuiro Mescco, Qaqarumicha. Poesía en castellano: Pável Ugarte Céspedes, Repatriación de las aves; Elvis David Quispe Altamirano, Visitame siempre en octubre; Martin Castillo Collado, Primera Dosis; Jhon Hansel Choque Condori, La Palabra no hace el amor, sino la ausencia</t>
-  </si>
-  <si>
     <t>img/Mujer_6_Libro5.jpg</t>
   </si>
   <si>
@@ -846,9 +793,6 @@
     <t>img/Mujer_6_Libro3.jpg</t>
   </si>
   <si>
-    <t>Centro de Estudios Constitucionales (CEC) Colección "Derecho y Sociedad" 2017</t>
-  </si>
-  <si>
     <t>https://www.tc.gob.pe/wp-content/uploads/2018/10/Justicia-e-interculturalidad.pdf</t>
   </si>
   <si>
@@ -880,6 +824,56 @@
   </si>
   <si>
     <t>Layo</t>
+  </si>
+  <si>
+    <t>Poesía (Quechua y Castellano). Antología de Ganadores de la Categoría “C” : Premio Regional de Cultura, 2015 / Dirección Desconcentrada de Cultura Cusco</t>
+  </si>
+  <si>
+    <t>(Antonieta realiza la corrección de estilo en quechua ). Antología de poemas en quechua y castellano de los ganadores de la Categoría “C”. Entre los poetas de esta antología tenemos: Gladis Naty Valencia Rosell, Huchuy harawikunata; Rocío Cjuiro Mescco, Qaqarumicha. Poesía en castellano: Pável Ugarte Céspedes, Repatriación de las aves; Elvis David Quispe Altamirano, Visitame siempre en octubre; Martin Castillo Collado, Primera Dosis; Jhon Hansel Choque Condori, La Palabra no hace el amor, sino la ausencia</t>
+  </si>
+  <si>
+    <t>Centro de Estudios Constitucionales (CEC) Colección  “Derecho y Sociedad” 2017</t>
+  </si>
+  <si>
+    <t>Adriana Cule es una artista visual y retratista profesional. Se desenvuelve en el terreno del diseño gráfico, el modelado análogo y digital, el desarrollo de personajes pintorescos y la creación de cuentos cortos. En sus obras busca que las perspectivas y composición interactúen con el espectador exagerando las formas.
+Ha participado en diferentes proyectos, muestras artísticas, diferentes campañas y producciones entre ellas la inauguración de Saga Falabella en Cusco, la filmación de Transformers en Cusco y la iniciativa de “Hagamos un Perú que de gusto” de Inca Kola.
+Ilustro el cuento “El zorro y el cóndor” de Maximo Ccama, realizo el libro de cuentos “Sueño Índigo” y los cómics “Pasado” y “Colores”.</t>
+  </si>
+  <si>
+    <t>Antología organizada por la Asociación Centro Cultural Cusco.</t>
+  </si>
+  <si>
+    <t>Éste es su primer poemario, como el título, un cúmulo de dulces y ácidas experiencias</t>
+  </si>
+  <si>
+    <t>Ana María Milla participa en esta antología con su poema en la página 349, esta publicación es una recopilación hecha por Alfred Asís Antología-Recopilación-Escritoras, Escritores-Poetas del Mundo.</t>
+  </si>
+  <si>
+    <t>El presente trabajo analiza la peregrinación de Sebastián “Quimichi”, a partir de la documentación que pertenece al archivo histórico del Santuario de Cocharcas, específicamente al documento denominado “Relación de la imagen de Nuestra Señora que está en este pueblo de Cocharca hecha por el licenciado don Pedro Guillén de Mendoza en 20 de julio de 1625 años”.</t>
+  </si>
+  <si>
+    <t>El presente artículo se enmarca en el difícil proceso de reorganización social y religiosa que las poblaciones indígenas padecieron dentro de la región de Huamanga en la coyuntura finisecular del siglo XVI. Nuestra preocupación por comprender dichas reorganizaciones obedece a un doble interés, primero dar cuenta de la conformación del espacio social de la doctrina de Cocharcas, y segundo realizar un análisis de las relaciones interétnicas y las nociones de inclusión/exclusión a partir de la implementación de la cofradía, convirtiéndose en el medio de mayor eficacia para canalizar y viabilizar los intereses colonial étnicos locales de poder para así ganarse un espacio dentro de la nueva sociedad colonial que se conformaba.</t>
+  </si>
+  <si>
+    <t>Gladys Conde es acreedora de mención honrosa en poesía por el Premio Regional de Cultura de Cusco (2006), publicándose sus poemas en “Antología Poética del Cusco” realizado por el INC en el 2007.</t>
+  </si>
+  <si>
+    <t>En el presente artículo la ilustradora explica: Lejos de proponer una visión romanizada de la tradición oral y la cosmovisión ancestral, pretendo brindar reflexiones desde mi práctica artística personal y desde la corriente estética del surrealismo sobre los elementos claves de la identidad y los ecosistemas en el Perú. Mucha de la influencia e inspiración nace tanto de artistas y artesanos locales como internacionales. Me enfoco en corrientes que nacieron en la colonia, como es la reconocida Escuela Cusqueña, que tiene como representantes a pintores como Diego Quispe Tito, o el pintor Italiano Bernardo Bitti. Cabe resaltar que los trabajos de la Escuela Cusqueña en mayoría son obras de pintores originarios y mestizos. Obras sacras como las del Corpus Christi siglo XVII de autor anónimo o la obra Virgen del Carmen del siglo XVII, que por su composición se asocia a la representación de la Pachamama, son importantes como antecedente de la pintura actual peruana enfocada en lo tradicional y la ecología</t>
+  </si>
+  <si>
+    <t>Con experiencia laboral desde el 2003 hasta la actualidad. Natalia Lizarraga ha trabajado en diferentes proyectos artísticos individuales y colectivos. Su trabajo consiste en estéticas como el surrealismo, surrealismo narrativo, que se ven reflejados en trabajos como: “Dulcinea”, “Huida a Egipto“, “Nativo“, parte del proyecto “Memoria 2014“ que constó de 4 exhibiciones realizadas en diferentes Centros Culturales del Cusco-Perú; otros trabajos con enfoque mayormente ecológico, de diferentes especies emblemáticas o en peligro de extinción a nivel nacional o internacional tenemos “Tigrillo“ 2015. Tambien en sus exposiciones se han enfocado en la cultura viva como son tradiciones orales, con obras como con la muestra realizada en la casa cultural Cusco-Perú , 2016. Otras expresiones artisticas que revalorando tradiciones y creencias mortuarios que se tienen en la actualidad que provienen desde la cosmovisión precolombina, con obras como “El condenado“, “Aparición“, “Ofrendas“ . Sobre mitos y leyendas, a nivel nacional e internacional nos deleita con obras como “El Minotauro“ 2004. Natalia Lizarraga ha tenido exposiciónes individuales y colectivas en el Perú como en el extranjero en paises como: México, Bruselas, Alemania y Estados Unidos. En el campo de la ilustración ha participando en proyecto como la publicación “Cuentos Aguarunas“ del Centro Guamán Poma de Ayala Cusco en 2010, tambien trabajo en el libro-cancionero “LLIQLLA“2021 con la Editorial SM Perú y colaborando en la portada del Álbum Musical Lliqlla de la misma cantautora Gladys Conde, Cusco, 2021.</t>
+  </si>
+  <si>
+    <t>Sueño Índigo</t>
+  </si>
+  <si>
+    <t>Antología Ángeles y Demonios</t>
+  </si>
+  <si>
+    <t>Mil Poemas a César Vallejo: Una gesta de amor universal</t>
+  </si>
+  <si>
+    <t>Cuentos Aguarunas</t>
   </si>
 </sst>
 </file>
@@ -889,11 +883,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -967,11 +968,6 @@
       <name val="&quot;Times New Roman&quot;"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="&quot;Times New Roman&quot;"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1029,17 +1025,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF4D5F72"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -1052,8 +1037,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4D5F72"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1120,8 +1111,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1173,19 +1170,6 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -1375,317 +1359,290 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2032,52 +1989,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94D338E-FEBE-4758-8002-AA19DAC4F902}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>93</v>
+      <c r="A1" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1">
-      <c r="A2" s="38">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>94</v>
+      <c r="B2" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1">
-      <c r="A3" s="107">
+      <c r="A3" s="90">
         <v>2</v>
       </c>
-      <c r="B3" s="108" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="108" t="s">
-        <v>251</v>
-      </c>
-      <c r="D3" s="108" t="s">
-        <v>252</v>
+      <c r="B3" s="91" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="91" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="91" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -2089,8 +2046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2100,7 +2057,9 @@
     <col min="3" max="3" width="14.81640625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="19.453125" customWidth="1"/>
-    <col min="6" max="8" width="20.453125" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" customWidth="1"/>
+    <col min="7" max="7" width="69.453125" customWidth="1"/>
+    <col min="8" max="8" width="20.453125" customWidth="1"/>
     <col min="9" max="9" width="35.453125" customWidth="1"/>
     <col min="10" max="10" width="21.36328125" customWidth="1"/>
     <col min="11" max="11" width="21.54296875" customWidth="1"/>
@@ -2108,257 +2067,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>112</v>
+      <c r="I1" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="78" customHeight="1" thickBot="1">
-      <c r="A2" s="19">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="17">
         <v>1</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="18">
         <v>35175</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="21" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="95" t="s">
+        <v>238</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="J2" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="78" customHeight="1" thickBot="1">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="17">
+        <v>1</v>
+      </c>
+      <c r="E3" s="22">
+        <v>28291</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="78" customHeight="1" thickBot="1">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="17">
+        <v>1</v>
+      </c>
+      <c r="E4" s="24">
+        <v>29378</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="L4" s="42" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="61.5" customHeight="1" thickBot="1">
+      <c r="A5" s="35">
+        <v>4</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="37">
+        <v>1</v>
+      </c>
+      <c r="E5" s="38">
+        <v>30017</v>
+      </c>
+      <c r="F5" s="36"/>
+      <c r="G5" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
+      <c r="A6" s="43">
+        <v>5</v>
+      </c>
+      <c r="B6" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="I2" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="46" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="78" customHeight="1" thickBot="1">
-      <c r="A3" s="19">
+      <c r="C6" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="45">
+        <v>1</v>
+      </c>
+      <c r="E6" s="46">
+        <v>30231</v>
+      </c>
+      <c r="F6" s="44"/>
+      <c r="G6" s="92" t="s">
+        <v>246</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="I6" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="J6" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="K6" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="L6" s="71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="53.5" customHeight="1" thickBot="1">
+      <c r="A7" s="72">
+        <v>6</v>
+      </c>
+      <c r="B7" s="73" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="74">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="19">
-        <v>1</v>
-      </c>
-      <c r="E3" s="24">
-        <v>28291</v>
-      </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="K3" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="L3" s="46" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="78" customHeight="1" thickBot="1">
-      <c r="A4" s="19">
-        <v>3</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="19">
-        <v>1</v>
-      </c>
-      <c r="E4" s="26">
-        <v>29378</v>
-      </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="K4" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="L4" s="46" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="61.5" customHeight="1" thickBot="1">
-      <c r="A5" s="39">
-        <v>4</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="D5" s="41">
-        <v>1</v>
-      </c>
-      <c r="E5" s="42">
-        <v>30017</v>
-      </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="43" t="s">
-        <v>154</v>
-      </c>
-      <c r="H5" s="44" t="s">
-        <v>155</v>
-      </c>
-      <c r="I5" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="J5" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="K5" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="L5" s="46" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A6" s="47">
-        <v>5</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>161</v>
-      </c>
-      <c r="D6" s="49">
-        <v>1</v>
-      </c>
-      <c r="E6" s="50">
-        <v>30231</v>
-      </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="51" t="s">
-        <v>196</v>
-      </c>
-      <c r="H6" s="52" t="s">
-        <v>162</v>
-      </c>
-      <c r="I6" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="J6" s="48" t="s">
-        <v>164</v>
-      </c>
-      <c r="K6" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="L6" s="87" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" thickBot="1">
-      <c r="A7" s="88">
-        <v>6</v>
-      </c>
-      <c r="B7" s="89" t="s">
-        <v>200</v>
-      </c>
-      <c r="C7" s="89" t="s">
-        <v>201</v>
-      </c>
-      <c r="D7" s="90">
-        <v>2</v>
-      </c>
-      <c r="E7" s="91">
+      <c r="E7" s="75">
         <v>29716</v>
       </c>
-      <c r="F7" s="89"/>
+      <c r="F7" s="73"/>
       <c r="G7" s="92" t="s">
-        <v>202</v>
-      </c>
-      <c r="H7" s="89" t="s">
-        <v>203</v>
-      </c>
-      <c r="I7" s="89" t="s">
-        <v>204</v>
-      </c>
-      <c r="J7" s="94" t="s">
-        <v>205</v>
-      </c>
-      <c r="K7" s="89" t="s">
-        <v>206</v>
-      </c>
-      <c r="L7" s="93" t="s">
-        <v>207</v>
+        <v>187</v>
+      </c>
+      <c r="H7" s="73" t="s">
+        <v>188</v>
+      </c>
+      <c r="I7" s="73" t="s">
+        <v>189</v>
+      </c>
+      <c r="J7" s="77" t="s">
+        <v>190</v>
+      </c>
+      <c r="K7" s="73" t="s">
+        <v>191</v>
+      </c>
+      <c r="L7" s="76" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2380,15 +2339,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="4.453125" customWidth="1"/>
     <col min="2" max="2" width="30.453125" customWidth="1"/>
-    <col min="3" max="4" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
     <col min="5" max="5" width="10.54296875" customWidth="1"/>
     <col min="6" max="6" width="56" customWidth="1"/>
     <col min="7" max="7" width="10.54296875" customWidth="1"/>
@@ -2396,1047 +2356,1047 @@
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.5">
+    <row r="1" spans="1:10" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="61.5" customHeight="1">
-      <c r="A2" s="30">
+        <v>92</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>26</v>
+      <c r="B2" s="93" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="93">
+        <v>9786124751028</v>
+      </c>
+      <c r="D2" s="97" t="s">
+        <v>53</v>
       </c>
       <c r="E2" s="8">
         <v>2018</v>
       </c>
-      <c r="F2" s="31" t="s">
-        <v>27</v>
+      <c r="F2" s="93" t="s">
+        <v>23</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="61.5" customHeight="1">
-      <c r="A3" s="30">
+        <v>108</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
+      <c r="A3" s="28">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="14">
+      <c r="B3" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="12">
         <v>2020</v>
       </c>
-      <c r="F3" s="32" t="s">
-        <v>30</v>
+      <c r="F3" s="94" t="s">
+        <v>26</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="61.5" customHeight="1">
-      <c r="A4" s="30">
+        <v>110</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
+      <c r="A4" s="28">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14" t="s">
+      <c r="B4" s="94" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="96"/>
+      <c r="D4" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="12">
+        <v>2021</v>
+      </c>
+      <c r="F4" s="94" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" s="14">
-        <v>2021</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>33</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="61.5" customHeight="1">
+        <v>110</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="15">
+      <c r="B5" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="96"/>
+      <c r="D5" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="13">
         <v>1998</v>
       </c>
-      <c r="F5" s="32" t="s">
-        <v>120</v>
+      <c r="F5" s="94" t="s">
+        <v>239</v>
       </c>
       <c r="G5" s="7">
         <v>2</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="J5" s="29"/>
-    </row>
-    <row r="6" spans="1:10" ht="29">
+        <v>124</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="J5" s="27"/>
+    </row>
+    <row r="6" spans="1:10" ht="31.5" thickBot="1">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="14">
+      <c r="B6" s="94" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="94">
         <v>200901791</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="15">
+      <c r="D6" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="13">
         <v>2009</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>63</v>
+      <c r="F6" s="94" t="s">
+        <v>240</v>
       </c>
       <c r="G6" s="7">
         <v>2</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="I6" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="J6" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="61.5" customHeight="1">
+        <v>125</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="15">
+      <c r="B7" s="94" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="96"/>
+      <c r="D7" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="13">
         <v>2012</v>
       </c>
-      <c r="F7" s="32" t="s">
-        <v>123</v>
+      <c r="F7" s="94" t="s">
+        <v>241</v>
       </c>
       <c r="G7" s="7">
         <v>2</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="I7" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="J7" s="34" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="61.5" customHeight="1">
+        <v>126</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="15">
+      <c r="B8" s="94" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="96"/>
+      <c r="D8" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="13">
         <v>2019</v>
       </c>
-      <c r="F8" s="32" t="s">
-        <v>67</v>
+      <c r="F8" s="94" t="s">
+        <v>58</v>
       </c>
       <c r="G8" s="7">
         <v>2</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="61.5" customHeight="1">
+        <v>108</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="15">
+      <c r="B9" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="96"/>
+      <c r="D9" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="13">
         <v>2019</v>
       </c>
-      <c r="F9" s="32" t="s">
-        <v>69</v>
+      <c r="F9" s="94" t="s">
+        <v>60</v>
       </c>
       <c r="G9" s="7">
         <v>2</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="J9" s="34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="61.5" customHeight="1">
+        <v>128</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="J9" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="14">
+      <c r="B10" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="94">
         <v>27098680</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="14">
+      <c r="D10" s="94" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="12">
         <v>2020</v>
       </c>
-      <c r="F10" s="32" t="s">
-        <v>37</v>
+      <c r="F10" s="94" t="s">
+        <v>242</v>
       </c>
       <c r="G10" s="3">
         <v>3</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="61.5" customHeight="1">
+        <v>129</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" s="31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="14">
+      <c r="B11" s="94" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="94">
         <v>287307</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="14">
+      <c r="D11" s="94" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" s="12">
         <v>2017</v>
       </c>
-      <c r="F11" s="32" t="s">
-        <v>39</v>
+      <c r="F11" s="94" t="s">
+        <v>34</v>
       </c>
       <c r="G11" s="3">
         <v>3</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="J11" s="35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="61.5" customHeight="1">
+        <v>130</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="83">
+      <c r="B12" s="94" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="94">
         <v>9786124544637</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="94" t="s">
+        <v>176</v>
+      </c>
+      <c r="E12" s="12">
+        <v>2013</v>
+      </c>
+      <c r="F12" s="94" t="s">
         <v>36</v>
-      </c>
-      <c r="E12" s="14">
-        <v>2013</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>41</v>
       </c>
       <c r="G12" s="3">
         <v>3</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="J12" s="35" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="61.5" customHeight="1">
+        <v>131</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="14">
+      <c r="B13" s="94" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="96"/>
+      <c r="D13" s="98" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="12">
         <v>2013</v>
       </c>
-      <c r="F13" s="32" t="s">
-        <v>43</v>
+      <c r="F13" s="94" t="s">
+        <v>243</v>
       </c>
       <c r="G13" s="3">
         <v>3</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="J13" s="35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="61.5" customHeight="1">
+        <v>132</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="14">
+      <c r="B14" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="96"/>
+      <c r="D14" s="94" t="s">
+        <v>176</v>
+      </c>
+      <c r="E14" s="12">
         <v>2014</v>
       </c>
-      <c r="F14" s="32"/>
+      <c r="F14" s="96"/>
       <c r="G14" s="3">
         <v>3</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="61.5" customHeight="1">
+        <v>115</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>49</v>
+      <c r="B15" s="94" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="96"/>
+      <c r="D15" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="94" t="s">
+        <v>43</v>
       </c>
       <c r="G15" s="3">
         <v>3</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="J15" s="36" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="61.5" customHeight="1">
+        <v>116</v>
+      </c>
+      <c r="J15" s="32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14" t="s">
+      <c r="B16" s="94" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="96"/>
+      <c r="D16" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="94" t="s">
         <v>47</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>53</v>
       </c>
       <c r="G16" s="3">
         <v>3</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="J16" s="37" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="61.5" customHeight="1">
+        <v>117</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="14">
+      <c r="B17" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="96"/>
+      <c r="D17" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="12">
         <v>2014</v>
       </c>
-      <c r="F17" s="32" t="s">
-        <v>55</v>
+      <c r="F17" s="94" t="s">
+        <v>49</v>
       </c>
       <c r="G17" s="3">
         <v>3</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="J17" s="37" t="s">
-        <v>129</v>
+        <v>117</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="61.5" customHeight="1" thickBot="1">
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>57</v>
+      <c r="B18" s="94" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="96"/>
+      <c r="D18" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="94" t="s">
+        <v>51</v>
       </c>
       <c r="G18" s="3">
         <v>3</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J18" s="34" t="s">
-        <v>58</v>
+        <v>120</v>
+      </c>
+      <c r="J18" s="30" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A19" s="53">
+      <c r="A19" s="48">
         <v>18</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="94" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="96"/>
+      <c r="D19" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="49">
+        <v>2007</v>
+      </c>
+      <c r="F19" s="94" t="s">
+        <v>244</v>
+      </c>
+      <c r="G19" s="50">
+        <v>4</v>
+      </c>
+      <c r="H19" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="I19" s="52" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" s="53" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A20" s="54">
+        <v>19</v>
+      </c>
+      <c r="B20" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="99">
+        <v>9786124544811</v>
+      </c>
+      <c r="D20" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="55">
+        <v>2009</v>
+      </c>
+      <c r="F20" s="94" t="s">
+        <v>159</v>
+      </c>
+      <c r="G20" s="56">
+        <v>4</v>
+      </c>
+      <c r="H20" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="I20" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="J20" s="58"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A21" s="54">
+        <v>20</v>
+      </c>
+      <c r="B21" s="94" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="99">
+        <v>9786123169701</v>
+      </c>
+      <c r="D21" s="94" t="s">
+        <v>162</v>
+      </c>
+      <c r="E21" s="55">
+        <v>2020</v>
+      </c>
+      <c r="F21" s="94" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" s="56">
+        <v>4</v>
+      </c>
+      <c r="H21" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="I21" s="52" t="s">
+        <v>108</v>
+      </c>
+      <c r="J21" s="60" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A22" s="54">
+        <v>21</v>
+      </c>
+      <c r="B22" s="94" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22" s="94">
+        <v>9786124456237</v>
+      </c>
+      <c r="D22" s="94" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="61">
+        <v>2020</v>
+      </c>
+      <c r="F22" s="94" t="s">
+        <v>166</v>
+      </c>
+      <c r="G22" s="62">
+        <v>4</v>
+      </c>
+      <c r="H22" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="56">
-        <v>2007</v>
-      </c>
-      <c r="F19" s="57" t="s">
+      <c r="I22" s="64" t="s">
         <v>168</v>
       </c>
-      <c r="G19" s="58">
-        <v>4</v>
-      </c>
-      <c r="H19" s="59" t="s">
+      <c r="J22" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="I19" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="J19" s="61" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A20" s="62">
-        <v>19</v>
-      </c>
-      <c r="B20" s="63" t="s">
+    </row>
+    <row r="23" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A23" s="65">
+        <v>22</v>
+      </c>
+      <c r="B23" s="94" t="s">
+        <v>250</v>
+      </c>
+      <c r="C23" s="94" t="s">
         <v>170</v>
       </c>
-      <c r="C20" s="64">
-        <v>9786124544811</v>
-      </c>
-      <c r="D20" s="65" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="66">
-        <v>2009</v>
-      </c>
-      <c r="F20" s="67" t="s">
+      <c r="D23" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="61">
+        <v>2010</v>
+      </c>
+      <c r="F23" s="94" t="s">
         <v>171</v>
       </c>
-      <c r="G20" s="68">
-        <v>4</v>
-      </c>
-      <c r="H20" s="59" t="s">
+      <c r="G23" s="61">
+        <v>5</v>
+      </c>
+      <c r="H23" s="58" t="s">
         <v>172</v>
       </c>
-      <c r="I20" s="69" t="s">
-        <v>121</v>
-      </c>
-      <c r="J20" s="70"/>
-    </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A21" s="62">
-        <v>20</v>
-      </c>
-      <c r="B21" s="63" t="s">
+      <c r="I23" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="C21" s="64">
-        <v>9786123169701</v>
-      </c>
-      <c r="D21" s="65" t="s">
+      <c r="J23" s="66" t="s">
         <v>174</v>
       </c>
-      <c r="E21" s="66">
+    </row>
+    <row r="24" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A24" s="65">
+        <v>23</v>
+      </c>
+      <c r="B24" s="94" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="96"/>
+      <c r="D24" s="94" t="s">
+        <v>176</v>
+      </c>
+      <c r="E24" s="61">
+        <v>2022</v>
+      </c>
+      <c r="F24" s="94" t="s">
+        <v>245</v>
+      </c>
+      <c r="G24" s="61">
+        <v>5</v>
+      </c>
+      <c r="H24" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="I24" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="J24" s="66" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A25" s="65">
+        <v>24</v>
+      </c>
+      <c r="B25" s="94" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="96">
+        <v>9786123270254</v>
+      </c>
+      <c r="D25" s="94" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" s="61">
         <v>2020</v>
       </c>
-      <c r="F21" s="67" t="s">
-        <v>175</v>
-      </c>
-      <c r="G21" s="68">
-        <v>4</v>
-      </c>
-      <c r="H21" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="I21" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="J21" s="72" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A22" s="62">
-        <v>21</v>
-      </c>
-      <c r="B22" s="73" t="s">
-        <v>177</v>
-      </c>
-      <c r="C22" s="74">
-        <v>9786124456237</v>
-      </c>
-      <c r="D22" s="65" t="s">
-        <v>174</v>
-      </c>
-      <c r="E22" s="74">
-        <v>2020</v>
-      </c>
-      <c r="F22" s="67" t="s">
-        <v>178</v>
-      </c>
-      <c r="G22" s="75">
-        <v>4</v>
-      </c>
-      <c r="H22" s="76" t="s">
-        <v>179</v>
-      </c>
-      <c r="I22" s="77" t="s">
+      <c r="F25" s="94" t="s">
         <v>180</v>
       </c>
-      <c r="J22" s="72" t="s">
+      <c r="G25" s="61">
+        <v>5</v>
+      </c>
+      <c r="H25" s="67" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A23" s="78">
-        <v>22</v>
-      </c>
-      <c r="B23" s="67" t="s">
-        <v>182</v>
-      </c>
-      <c r="C23" s="79" t="s">
-        <v>183</v>
-      </c>
-      <c r="D23" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="74">
-        <v>2010</v>
-      </c>
-      <c r="F23" s="67" t="s">
-        <v>184</v>
-      </c>
-      <c r="G23" s="74">
-        <v>5</v>
-      </c>
-      <c r="H23" s="70" t="s">
-        <v>185</v>
-      </c>
-      <c r="I23" s="70" t="s">
-        <v>186</v>
-      </c>
-      <c r="J23" s="80" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A24" s="78">
-        <v>23</v>
-      </c>
-      <c r="B24" s="67" t="s">
-        <v>188</v>
-      </c>
-      <c r="C24" s="70"/>
-      <c r="D24" s="67" t="s">
-        <v>189</v>
-      </c>
-      <c r="E24" s="74">
-        <v>2022</v>
-      </c>
-      <c r="F24" s="67" t="s">
-        <v>190</v>
-      </c>
-      <c r="G24" s="74">
-        <v>5</v>
-      </c>
-      <c r="H24" s="70" t="s">
-        <v>191</v>
-      </c>
-      <c r="I24" s="70" t="s">
-        <v>192</v>
-      </c>
-      <c r="J24" s="80" t="s">
+      <c r="I25" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="J25" s="59" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A26" s="78">
+        <v>25</v>
+      </c>
+      <c r="B26" s="94" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A25" s="78">
-        <v>24</v>
-      </c>
-      <c r="B25" s="67" t="s">
-        <v>173</v>
-      </c>
-      <c r="C25" s="81">
-        <v>9786123270254</v>
-      </c>
-      <c r="D25" s="67" t="s">
-        <v>174</v>
-      </c>
-      <c r="E25" s="74">
-        <v>2020</v>
-      </c>
-      <c r="F25" s="67" t="s">
+      <c r="C26" s="94">
+        <v>9789995415914</v>
+      </c>
+      <c r="D26" s="94" t="s">
         <v>194</v>
       </c>
-      <c r="G25" s="74">
-        <v>5</v>
-      </c>
-      <c r="H25" s="82" t="s">
+      <c r="E26" s="79">
+        <v>2014</v>
+      </c>
+      <c r="F26" s="94" t="s">
         <v>195</v>
       </c>
-      <c r="I25" s="70" t="s">
-        <v>117</v>
-      </c>
-      <c r="J25" s="71" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A26" s="95">
-        <v>25</v>
-      </c>
-      <c r="B26" s="96" t="s">
+      <c r="G26" s="79">
+        <v>6</v>
+      </c>
+      <c r="H26" s="79" t="s">
+        <v>196</v>
+      </c>
+      <c r="I26" s="79" t="s">
+        <v>197</v>
+      </c>
+      <c r="J26" s="53" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A27" s="80">
+        <v>26</v>
+      </c>
+      <c r="B27" s="94" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" s="94">
+        <v>9786124686528</v>
+      </c>
+      <c r="D27" s="94" t="s">
+        <v>200</v>
+      </c>
+      <c r="E27" s="81">
+        <v>2014</v>
+      </c>
+      <c r="F27" s="94" t="s">
+        <v>201</v>
+      </c>
+      <c r="G27" s="81">
+        <v>6</v>
+      </c>
+      <c r="H27" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="I27" s="81" t="s">
+        <v>203</v>
+      </c>
+      <c r="J27" s="60" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A28" s="80">
+        <v>27</v>
+      </c>
+      <c r="B28" s="94" t="s">
+        <v>235</v>
+      </c>
+      <c r="C28" s="94" t="s">
+        <v>205</v>
+      </c>
+      <c r="D28" s="94" t="s">
+        <v>200</v>
+      </c>
+      <c r="E28" s="81">
+        <v>2015</v>
+      </c>
+      <c r="F28" s="94" t="s">
+        <v>236</v>
+      </c>
+      <c r="G28" s="81">
+        <v>6</v>
+      </c>
+      <c r="H28" s="81" t="s">
+        <v>206</v>
+      </c>
+      <c r="I28" s="81" t="s">
+        <v>203</v>
+      </c>
+      <c r="J28" s="83"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A29" s="80">
+        <v>28</v>
+      </c>
+      <c r="B29" s="94" t="s">
+        <v>207</v>
+      </c>
+      <c r="C29" s="94">
+        <v>9789568416461</v>
+      </c>
+      <c r="D29" s="94" t="s">
         <v>208</v>
       </c>
-      <c r="C26" s="96">
-        <v>9789995415914</v>
-      </c>
-      <c r="D26" s="96" t="s">
+      <c r="E29" s="81">
+        <v>2016</v>
+      </c>
+      <c r="F29" s="94" t="s">
         <v>209</v>
       </c>
-      <c r="E26" s="96">
-        <v>2014</v>
-      </c>
-      <c r="F26" s="96" t="s">
+      <c r="G29" s="81">
+        <v>6</v>
+      </c>
+      <c r="H29" s="81" t="s">
         <v>210</v>
       </c>
-      <c r="G26" s="96">
+      <c r="I29" s="81" t="s">
+        <v>211</v>
+      </c>
+      <c r="J29" s="60" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A30" s="80">
+        <v>29</v>
+      </c>
+      <c r="B30" s="94" t="s">
+        <v>213</v>
+      </c>
+      <c r="C30" s="94">
+        <v>9789569853104</v>
+      </c>
+      <c r="D30" s="94" t="s">
+        <v>214</v>
+      </c>
+      <c r="E30" s="81">
+        <v>2017</v>
+      </c>
+      <c r="F30" s="94" t="s">
+        <v>215</v>
+      </c>
+      <c r="G30" s="81">
         <v>6</v>
       </c>
-      <c r="H26" s="96" t="s">
-        <v>211</v>
-      </c>
-      <c r="I26" s="96" t="s">
-        <v>212</v>
-      </c>
-      <c r="J26" s="61" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A27" s="97">
-        <v>26</v>
-      </c>
-      <c r="B27" s="98" t="s">
-        <v>214</v>
-      </c>
-      <c r="C27" s="98">
-        <v>9786124686528</v>
-      </c>
-      <c r="D27" s="98" t="s">
-        <v>215</v>
-      </c>
-      <c r="E27" s="98">
-        <v>2014</v>
-      </c>
-      <c r="F27" s="98" t="s">
+      <c r="H30" s="81" t="s">
         <v>216</v>
       </c>
-      <c r="G27" s="98">
+      <c r="I30" s="81" t="s">
+        <v>108</v>
+      </c>
+      <c r="J30" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A31" s="80">
+        <v>30</v>
+      </c>
+      <c r="B31" s="94" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" s="94"/>
+      <c r="D31" s="94" t="s">
+        <v>200</v>
+      </c>
+      <c r="E31" s="81">
+        <v>2018</v>
+      </c>
+      <c r="F31" s="94" t="s">
+        <v>218</v>
+      </c>
+      <c r="G31" s="81">
         <v>6</v>
       </c>
-      <c r="H27" s="98" t="s">
-        <v>217</v>
-      </c>
-      <c r="I27" s="98" t="s">
-        <v>218</v>
-      </c>
-      <c r="J27" s="72" t="s">
+      <c r="H31" s="81" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A28" s="97">
-        <v>27</v>
-      </c>
-      <c r="B28" s="98" t="s">
+      <c r="I31" s="81" t="s">
         <v>220</v>
       </c>
-      <c r="C28" s="98" t="s">
+      <c r="J31" s="83"/>
+    </row>
+    <row r="32" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A32" s="80">
+        <v>31</v>
+      </c>
+      <c r="B32" s="94" t="s">
         <v>221</v>
       </c>
-      <c r="D28" s="98" t="s">
-        <v>215</v>
-      </c>
-      <c r="E28" s="98">
-        <v>2015</v>
-      </c>
-      <c r="F28" s="98" t="s">
+      <c r="C32" s="94">
+        <v>9786124740831</v>
+      </c>
+      <c r="D32" s="94" t="s">
+        <v>208</v>
+      </c>
+      <c r="E32" s="81">
+        <v>2018</v>
+      </c>
+      <c r="F32" s="94" t="s">
         <v>222</v>
       </c>
-      <c r="G28" s="98">
+      <c r="G32" s="81">
         <v>6</v>
       </c>
-      <c r="H28" s="98" t="s">
+      <c r="H32" s="81" t="s">
         <v>223</v>
       </c>
-      <c r="I28" s="98" t="s">
-        <v>218</v>
-      </c>
-      <c r="J28" s="100"/>
-    </row>
-    <row r="29" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A29" s="97">
-        <v>28</v>
-      </c>
-      <c r="B29" s="98" t="s">
+      <c r="I32" s="81" t="s">
+        <v>237</v>
+      </c>
+      <c r="J32" s="60" t="s">
         <v>224</v>
       </c>
-      <c r="C29" s="98">
-        <v>9789568416461</v>
-      </c>
-      <c r="D29" s="98" t="s">
+    </row>
+    <row r="33" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A33" s="80">
+        <v>32</v>
+      </c>
+      <c r="B33" s="94" t="s">
         <v>225</v>
       </c>
-      <c r="E29" s="98">
-        <v>2016</v>
-      </c>
-      <c r="F29" s="98" t="s">
+      <c r="C33" s="94">
+        <v>9786124770265</v>
+      </c>
+      <c r="D33" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="81">
+        <v>2018</v>
+      </c>
+      <c r="F33" s="94" t="s">
         <v>226</v>
       </c>
-      <c r="G29" s="98">
+      <c r="G33" s="81">
         <v>6</v>
       </c>
-      <c r="H29" s="98" t="s">
+      <c r="H33" s="81" t="s">
         <v>227</v>
       </c>
-      <c r="I29" s="98" t="s">
+      <c r="I33" s="81" t="s">
+        <v>220</v>
+      </c>
+      <c r="J33" s="84"/>
+    </row>
+    <row r="34" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="A34" s="80">
+        <v>33</v>
+      </c>
+      <c r="B34" s="94" t="s">
         <v>228</v>
       </c>
-      <c r="J29" s="72" t="s">
+      <c r="C34" s="96"/>
+      <c r="D34" s="96" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A30" s="97">
-        <v>29</v>
-      </c>
-      <c r="B30" s="98" t="s">
+      <c r="E34" s="85">
+        <v>2012</v>
+      </c>
+      <c r="F34" s="96" t="s">
         <v>230</v>
       </c>
-      <c r="C30" s="98">
-        <v>9789569853104</v>
-      </c>
-      <c r="D30" s="98" t="s">
+      <c r="G34" s="81">
+        <v>6</v>
+      </c>
+      <c r="H34" s="81" t="s">
         <v>231</v>
       </c>
-      <c r="E30" s="98">
-        <v>2017</v>
-      </c>
-      <c r="F30" s="98" t="s">
-        <v>232</v>
-      </c>
-      <c r="G30" s="98">
-        <v>6</v>
-      </c>
-      <c r="H30" s="98" t="s">
-        <v>233</v>
-      </c>
-      <c r="I30" s="98" t="s">
-        <v>117</v>
-      </c>
-      <c r="J30" s="99" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A31" s="97">
-        <v>30</v>
-      </c>
-      <c r="B31" s="98" t="s">
-        <v>234</v>
-      </c>
-      <c r="C31" s="98"/>
-      <c r="D31" s="98" t="s">
-        <v>215</v>
-      </c>
-      <c r="E31" s="98">
-        <v>2018</v>
-      </c>
-      <c r="F31" s="98" t="s">
-        <v>235</v>
-      </c>
-      <c r="G31" s="98">
-        <v>6</v>
-      </c>
-      <c r="H31" s="98" t="s">
-        <v>236</v>
-      </c>
-      <c r="I31" s="98" t="s">
-        <v>237</v>
-      </c>
-      <c r="J31" s="100"/>
-    </row>
-    <row r="32" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A32" s="97">
-        <v>31</v>
-      </c>
-      <c r="B32" s="98" t="s">
-        <v>238</v>
-      </c>
-      <c r="C32" s="98">
-        <v>9786124740831</v>
-      </c>
-      <c r="D32" s="98" t="s">
-        <v>225</v>
-      </c>
-      <c r="E32" s="98">
-        <v>2018</v>
-      </c>
-      <c r="F32" s="98" t="s">
-        <v>239</v>
-      </c>
-      <c r="G32" s="98">
-        <v>6</v>
-      </c>
-      <c r="H32" s="98" t="s">
-        <v>240</v>
-      </c>
-      <c r="I32" s="98" t="s">
-        <v>241</v>
-      </c>
-      <c r="J32" s="72" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A33" s="97">
-        <v>32</v>
-      </c>
-      <c r="B33" s="98" t="s">
-        <v>243</v>
-      </c>
-      <c r="C33" s="98">
-        <v>9786124770265</v>
-      </c>
-      <c r="D33" s="98" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" s="98">
-        <v>2018</v>
-      </c>
-      <c r="F33" s="98" t="s">
-        <v>244</v>
-      </c>
-      <c r="G33" s="98">
-        <v>6</v>
-      </c>
-      <c r="H33" s="98" t="s">
-        <v>245</v>
-      </c>
-      <c r="I33" s="98" t="s">
-        <v>237</v>
-      </c>
-      <c r="J33" s="101"/>
-    </row>
-    <row r="34" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A34" s="97">
-        <v>33</v>
-      </c>
-      <c r="B34" s="98" t="s">
-        <v>246</v>
-      </c>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100" t="s">
-        <v>247</v>
-      </c>
-      <c r="E34" s="102">
-        <v>2012</v>
-      </c>
-      <c r="F34" s="100" t="s">
-        <v>248</v>
-      </c>
-      <c r="G34" s="98">
-        <v>6</v>
-      </c>
-      <c r="H34" s="98" t="s">
-        <v>249</v>
-      </c>
-      <c r="I34" s="98" t="s">
-        <v>237</v>
-      </c>
-      <c r="J34" s="99"/>
+      <c r="I34" s="81" t="s">
+        <v>220</v>
+      </c>
+      <c r="J34" s="82"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3487,102 +3447,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>77</v>
+      <c r="B1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" thickBot="1">
-      <c r="A2" s="84">
+      <c r="A2" s="68">
         <v>1</v>
       </c>
-      <c r="B2" s="84">
+      <c r="B2" s="68">
         <v>1</v>
       </c>
-      <c r="C2" s="85" t="s">
-        <v>73</v>
+      <c r="C2" s="69" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" thickBot="1">
-      <c r="A3" s="84">
+      <c r="A3" s="68">
         <v>2</v>
       </c>
-      <c r="B3" s="84">
+      <c r="B3" s="68">
         <v>1</v>
       </c>
-      <c r="C3" s="85" t="s">
-        <v>72</v>
+      <c r="C3" s="69" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3" thickBot="1">
-      <c r="A4" s="84">
+      <c r="A4" s="68">
         <v>3</v>
       </c>
-      <c r="B4" s="84">
+      <c r="B4" s="68">
         <v>1</v>
       </c>
-      <c r="C4" s="85" t="s">
-        <v>71</v>
+      <c r="C4" s="69" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" thickBot="1">
-      <c r="A5" s="84">
+      <c r="A5" s="68">
         <v>4</v>
       </c>
-      <c r="B5" s="84">
+      <c r="B5" s="68">
         <v>2</v>
       </c>
-      <c r="C5" s="85" t="s">
-        <v>75</v>
+      <c r="C5" s="69" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" thickBot="1">
-      <c r="A6" s="84">
+      <c r="A6" s="68">
         <v>5</v>
       </c>
-      <c r="B6" s="84">
+      <c r="B6" s="68">
         <v>2</v>
       </c>
-      <c r="C6" s="85" t="s">
-        <v>72</v>
+      <c r="C6" s="69" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" thickBot="1">
-      <c r="A7" s="84">
+      <c r="A7" s="68">
         <v>6</v>
       </c>
-      <c r="B7" s="84">
+      <c r="B7" s="68">
         <v>3</v>
       </c>
-      <c r="C7" s="85" t="s">
-        <v>87</v>
+      <c r="C7" s="69" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A8" s="84">
+      <c r="A8" s="68">
         <v>7</v>
       </c>
-      <c r="B8" s="84">
+      <c r="B8" s="68">
         <v>3</v>
       </c>
-      <c r="C8" s="85" t="s">
-        <v>74</v>
+      <c r="C8" s="69" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A9" s="84">
+      <c r="A9" s="68">
         <v>8</v>
       </c>
-      <c r="B9" s="84">
+      <c r="B9" s="68">
         <v>4</v>
       </c>
-      <c r="C9" s="85" t="s">
-        <v>75</v>
+      <c r="C9" s="69" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
@@ -3592,52 +3552,52 @@
       <c r="B10">
         <v>5</v>
       </c>
-      <c r="C10" s="86" t="s">
-        <v>73</v>
+      <c r="C10" s="70" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A11" s="103">
+      <c r="A11" s="86">
         <v>10</v>
       </c>
-      <c r="B11" s="103">
+      <c r="B11" s="86">
         <v>6</v>
       </c>
-      <c r="C11" s="104" t="s">
-        <v>72</v>
+      <c r="C11" s="87" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A12" s="103">
+      <c r="A12" s="86">
         <v>11</v>
       </c>
-      <c r="B12" s="103">
+      <c r="B12" s="86">
         <v>6</v>
       </c>
-      <c r="C12" s="104" t="s">
-        <v>74</v>
+      <c r="C12" s="87" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A13" s="103">
+      <c r="A13" s="86">
         <v>12</v>
       </c>
-      <c r="B13" s="103">
+      <c r="B13" s="86">
         <v>6</v>
       </c>
-      <c r="C13" s="104" t="s">
-        <v>250</v>
+      <c r="C13" s="87" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A14" s="105">
+      <c r="A14" s="88">
         <v>13</v>
       </c>
-      <c r="B14" s="105">
+      <c r="B14" s="88">
         <v>6</v>
       </c>
-      <c r="C14" s="106" t="s">
-        <v>80</v>
+      <c r="C14" s="89" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1"/>
@@ -4546,83 +4506,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.5">
+      <c r="A2" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.5">
+      <c r="A3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.5">
+      <c r="A4" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.5">
+      <c r="A5" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.5">
+      <c r="A6" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.5">
+      <c r="A7" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.5">
+      <c r="A8" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.5">
-      <c r="A2" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.5">
-      <c r="A3" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.5">
-      <c r="A4" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.5">
-      <c r="A5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14.5">
-      <c r="A6" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="14.5">
-      <c r="A7" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="14.5">
-      <c r="A8" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Natalya y libro N19
</commit_message>
<xml_diff>
--- a/CR/11_05_22BasedeDatosMDLPcorrect.xlsx
+++ b/CR/11_05_22BasedeDatosMDLPcorrect.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\Documents\PaginaWebCusco\CR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1949F756-0B82-4F89-B717-FD814C46D64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064A6B5C-4A21-449A-870C-24CE1AF09AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lugar" sheetId="6" r:id="rId1"/>
@@ -566,9 +566,6 @@
     <t>https://www.youtube.com/embed/myEpMpTkVSY</t>
   </si>
   <si>
-    <t>Natalia Eddem</t>
-  </si>
-  <si>
     <t>Lizarraga Conchatupa</t>
   </si>
   <si>
@@ -594,9 +591,6 @@
   </si>
   <si>
     <t>Juego y silencio</t>
-  </si>
-  <si>
-    <t>Gladys Conde ha bebido de la fuente de nuestros ancestros para crear estas maravillosas canciones para el arrullo y el sueño; para crecer y sanar. Los once cantos que incluye este libro nos hacen contemplar la armonía cósmica que reina entre plantas y animales; entre el cielo y la tierra. Las canciones además vienen acompañadas de las luminosas pinturas de la artista plástica Natalya Lizárraga.</t>
   </si>
   <si>
     <t>img/Mujer_4_Libro2.jpg</t>
@@ -861,9 +855,6 @@
     <t>En el presente artículo la ilustradora explica: Lejos de proponer una visión romanizada de la tradición oral y la cosmovisión ancestral, pretendo brindar reflexiones desde mi práctica artística personal y desde la corriente estética del surrealismo sobre los elementos claves de la identidad y los ecosistemas en el Perú. Mucha de la influencia e inspiración nace tanto de artistas y artesanos locales como internacionales. Me enfoco en corrientes que nacieron en la colonia, como es la reconocida Escuela Cusqueña, que tiene como representantes a pintores como Diego Quispe Tito, o el pintor Italiano Bernardo Bitti. Cabe resaltar que los trabajos de la Escuela Cusqueña en mayoría son obras de pintores originarios y mestizos. Obras sacras como las del Corpus Christi siglo XVII de autor anónimo o la obra Virgen del Carmen del siglo XVII, que por su composición se asocia a la representación de la Pachamama, son importantes como antecedente de la pintura actual peruana enfocada en lo tradicional y la ecología</t>
   </si>
   <si>
-    <t>Con experiencia laboral desde el 2003 hasta la actualidad. Natalia Lizarraga ha trabajado en diferentes proyectos artísticos individuales y colectivos. Su trabajo consiste en estéticas como el surrealismo, surrealismo narrativo, que se ven reflejados en trabajos como: “Dulcinea”, “Huida a Egipto“, “Nativo“, parte del proyecto “Memoria 2014“ que constó de 4 exhibiciones realizadas en diferentes Centros Culturales del Cusco-Perú; otros trabajos con enfoque mayormente ecológico, de diferentes especies emblemáticas o en peligro de extinción a nivel nacional o internacional tenemos “Tigrillo“ 2015. Tambien en sus exposiciones se han enfocado en la cultura viva como son tradiciones orales, con obras como con la muestra realizada en la casa cultural Cusco-Perú , 2016. Otras expresiones artisticas que revalorando tradiciones y creencias mortuarios que se tienen en la actualidad que provienen desde la cosmovisión precolombina, con obras como “El condenado“, “Aparición“, “Ofrendas“ . Sobre mitos y leyendas, a nivel nacional e internacional nos deleita con obras como “El Minotauro“ 2004. Natalia Lizarraga ha tenido exposiciónes individuales y colectivas en el Perú como en el extranjero en paises como: México, Bruselas, Alemania y Estados Unidos. En el campo de la ilustración ha participando en proyecto como la publicación “Cuentos Aguarunas“ del Centro Guamán Poma de Ayala Cusco en 2010, tambien trabajo en el libro-cancionero “LLIQLLA“2021 con la Editorial SM Perú y colaborando en la portada del Álbum Musical Lliqlla de la misma cantautora Gladys Conde, Cusco, 2021.</t>
-  </si>
-  <si>
     <t>Sueño Índigo</t>
   </si>
   <si>
@@ -874,6 +865,15 @@
   </si>
   <si>
     <t>Cuentos Aguarunas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natalya Eddem </t>
+  </si>
+  <si>
+    <t>Con experiencia laboral desde el 2003 hasta la actualidad. Natalya Lizarraga ha trabajado en diferentes proyectos artísticos individuales y colectivos. Su trabajo consiste en estéticas como el surrealismo, surrealismo narrativo, que se ven reflejados en trabajos como: “Dulcinea”, “Huida a Egipto“, “Nativo“, parte del proyecto “Memoria 2014“ que constó de 4 exhibiciones realizadas en diferentes Centros Culturales del Cusco-Perú; otros trabajos con enfoque mayormente ecológico, de diferentes especies emblemáticas o en peligro de extinción a nivel nacional o internacional tenemos “Tigrillo“ 2015. Tambien en sus exposiciones se han enfocado en la cultura viva como son tradiciones orales, con obras como con la muestra realizada en la casa cultural Cusco-Perú , 2016. Otras expresiones artisticas que revalorando tradiciones y creencias mortuarios que se tienen en la actualidad que provienen desde la cosmovisión precolombina, con obras como “El condenado“, “Aparición“, “Ofrendas“ . Sobre mitos y leyendas, a nivel nacional e internacional nos deleita con obras como “El Minotauro“ 2004. Natalia Lizarraga ha tenido exposiciónes individuales y colectivas en el Perú como en el extranjero en paises como: México, Bruselas, Alemania y Estados Unidos. En el campo de la ilustración ha participando en proyecto como la publicación “Cuentos Aguarunas“ del Centro Guamán Poma de Ayala Cusco en 2010, tambien trabajo en el libro-cancionero “LLIQLLA“2021 con la Editorial SM Perú y colaborando en la portada del Álbum Musical Lliqlla de la misma cantautora Gladys Conde, Cusco, 2021.</t>
+  </si>
+  <si>
+    <t>Poemario de 26 poemas cortos, algunos lúdicos otros más serios; donde la poeta relaciona el proceso de creer con metaforas de la naturaleza, el juego y el silencio.</t>
   </si>
 </sst>
 </file>
@@ -883,11 +883,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1357,293 +1364,296 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2031,10 +2041,10 @@
         <v>85</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D3" s="91" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2047,7 +2057,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2122,7 +2132,7 @@
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="95" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>138</v>
@@ -2137,7 +2147,7 @@
         <v>87</v>
       </c>
       <c r="L2" s="42" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="78" customHeight="1" thickBot="1">
@@ -2173,7 +2183,7 @@
         <v>105</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="78" customHeight="1" thickBot="1">
@@ -2209,7 +2219,7 @@
         <v>107</v>
       </c>
       <c r="L4" s="42" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="61.5" customHeight="1" thickBot="1">
@@ -2252,11 +2262,11 @@
       <c r="A6" s="43">
         <v>5</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="100" t="s">
+        <v>248</v>
+      </c>
+      <c r="C6" s="44" t="s">
         <v>149</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>150</v>
       </c>
       <c r="D6" s="45">
         <v>1</v>
@@ -2265,23 +2275,23 @@
         <v>30231</v>
       </c>
       <c r="F6" s="44"/>
-      <c r="G6" s="92" t="s">
-        <v>246</v>
+      <c r="G6" s="101" t="s">
+        <v>249</v>
       </c>
       <c r="H6" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="I6" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="I6" s="44" t="s">
+      <c r="J6" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="K6" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="K6" s="40" t="s">
+      <c r="L6" s="71" t="s">
         <v>154</v>
-      </c>
-      <c r="L6" s="71" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="53.5" customHeight="1" thickBot="1">
@@ -2289,10 +2299,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="73" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C7" s="73" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D7" s="74">
         <v>2</v>
@@ -2302,22 +2312,22 @@
       </c>
       <c r="F7" s="73"/>
       <c r="G7" s="92" t="s">
+        <v>185</v>
+      </c>
+      <c r="H7" s="73" t="s">
+        <v>186</v>
+      </c>
+      <c r="I7" s="73" t="s">
         <v>187</v>
       </c>
-      <c r="H7" s="73" t="s">
+      <c r="J7" s="77" t="s">
         <v>188</v>
       </c>
-      <c r="I7" s="73" t="s">
+      <c r="K7" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="J7" s="77" t="s">
+      <c r="L7" s="76" t="s">
         <v>190</v>
-      </c>
-      <c r="K7" s="73" t="s">
-        <v>191</v>
-      </c>
-      <c r="L7" s="76" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2339,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2393,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="93" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C2" s="93">
         <v>9786124751028</v>
@@ -2485,7 +2495,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="94" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C5" s="96"/>
       <c r="D5" s="94" t="s">
@@ -2495,7 +2505,7 @@
         <v>1998</v>
       </c>
       <c r="F5" s="94" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G5" s="7">
         <v>2</v>
@@ -2525,7 +2535,7 @@
         <v>2009</v>
       </c>
       <c r="F6" s="94" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G6" s="7">
         <v>2</v>
@@ -2545,7 +2555,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="94" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C7" s="96"/>
       <c r="D7" s="94" t="s">
@@ -2555,7 +2565,7 @@
         <v>2012</v>
       </c>
       <c r="F7" s="94" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G7" s="7">
         <v>2</v>
@@ -2641,13 +2651,13 @@
         <v>27098680</v>
       </c>
       <c r="D10" s="94" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E10" s="12">
         <v>2020</v>
       </c>
       <c r="F10" s="94" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G10" s="3">
         <v>3</v>
@@ -2673,7 +2683,7 @@
         <v>287307</v>
       </c>
       <c r="D11" s="94" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E11" s="12">
         <v>2017</v>
@@ -2705,7 +2715,7 @@
         <v>9786124544637</v>
       </c>
       <c r="D12" s="94" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E12" s="12">
         <v>2013</v>
@@ -2741,7 +2751,7 @@
         <v>2013</v>
       </c>
       <c r="F13" s="94" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G13" s="3">
         <v>3</v>
@@ -2765,7 +2775,7 @@
       </c>
       <c r="C14" s="96"/>
       <c r="D14" s="94" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E14" s="12">
         <v>2014</v>
@@ -2909,7 +2919,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="94" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C19" s="96"/>
       <c r="D19" s="94" t="s">
@@ -2919,13 +2929,13 @@
         <v>2007</v>
       </c>
       <c r="F19" s="94" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G19" s="50">
         <v>4</v>
       </c>
       <c r="H19" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I19" s="52" t="s">
         <v>108</v>
@@ -2939,7 +2949,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="94" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C20" s="99">
         <v>9786124544811</v>
@@ -2950,14 +2960,14 @@
       <c r="E20" s="55">
         <v>2009</v>
       </c>
-      <c r="F20" s="94" t="s">
-        <v>159</v>
+      <c r="F20" s="102" t="s">
+        <v>250</v>
       </c>
       <c r="G20" s="56">
         <v>4</v>
       </c>
       <c r="H20" s="51" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I20" s="57" t="s">
         <v>111</v>
@@ -2969,25 +2979,25 @@
         <v>20</v>
       </c>
       <c r="B21" s="94" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C21" s="99">
         <v>9786123169701</v>
       </c>
       <c r="D21" s="94" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E21" s="55">
         <v>2020</v>
       </c>
       <c r="F21" s="94" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G21" s="56">
         <v>4</v>
       </c>
       <c r="H21" s="51" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I21" s="52" t="s">
         <v>108</v>
@@ -3001,31 +3011,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="94" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C22" s="94">
         <v>9786124456237</v>
       </c>
       <c r="D22" s="94" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E22" s="61">
         <v>2020</v>
       </c>
       <c r="F22" s="94" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G22" s="62">
         <v>4</v>
       </c>
       <c r="H22" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="64" t="s">
+        <v>166</v>
+      </c>
+      <c r="J22" s="60" t="s">
         <v>167</v>
-      </c>
-      <c r="I22" s="64" t="s">
-        <v>168</v>
-      </c>
-      <c r="J22" s="60" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" thickBot="1">
@@ -3033,10 +3043,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="94" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C23" s="94" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D23" s="94" t="s">
         <v>53</v>
@@ -3045,19 +3055,19 @@
         <v>2010</v>
       </c>
       <c r="F23" s="94" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G23" s="61">
         <v>5</v>
       </c>
       <c r="H23" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="I23" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="J23" s="66" t="s">
         <v>172</v>
-      </c>
-      <c r="I23" s="58" t="s">
-        <v>173</v>
-      </c>
-      <c r="J23" s="66" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" thickBot="1">
@@ -3065,29 +3075,29 @@
         <v>23</v>
       </c>
       <c r="B24" s="94" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C24" s="96"/>
       <c r="D24" s="94" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E24" s="61">
         <v>2022</v>
       </c>
       <c r="F24" s="94" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G24" s="61">
         <v>5</v>
       </c>
       <c r="H24" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="I24" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="J24" s="66" t="s">
         <v>177</v>
-      </c>
-      <c r="I24" s="58" t="s">
-        <v>178</v>
-      </c>
-      <c r="J24" s="66" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" thickBot="1">
@@ -3095,25 +3105,25 @@
         <v>24</v>
       </c>
       <c r="B25" s="94" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C25" s="96">
         <v>9786123270254</v>
       </c>
       <c r="D25" s="94" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E25" s="61">
         <v>2020</v>
       </c>
       <c r="F25" s="94" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G25" s="61">
         <v>5</v>
       </c>
       <c r="H25" s="67" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I25" s="58" t="s">
         <v>108</v>
@@ -3127,31 +3137,31 @@
         <v>25</v>
       </c>
       <c r="B26" s="94" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C26" s="94">
         <v>9789995415914</v>
       </c>
       <c r="D26" s="94" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E26" s="79">
         <v>2014</v>
       </c>
       <c r="F26" s="94" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G26" s="79">
         <v>6</v>
       </c>
       <c r="H26" s="79" t="s">
+        <v>194</v>
+      </c>
+      <c r="I26" s="79" t="s">
+        <v>195</v>
+      </c>
+      <c r="J26" s="53" t="s">
         <v>196</v>
-      </c>
-      <c r="I26" s="79" t="s">
-        <v>197</v>
-      </c>
-      <c r="J26" s="53" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" thickBot="1">
@@ -3159,31 +3169,31 @@
         <v>26</v>
       </c>
       <c r="B27" s="94" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C27" s="94">
         <v>9786124686528</v>
       </c>
       <c r="D27" s="94" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E27" s="81">
         <v>2014</v>
       </c>
       <c r="F27" s="94" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G27" s="81">
         <v>6</v>
       </c>
       <c r="H27" s="81" t="s">
+        <v>200</v>
+      </c>
+      <c r="I27" s="81" t="s">
+        <v>201</v>
+      </c>
+      <c r="J27" s="60" t="s">
         <v>202</v>
-      </c>
-      <c r="I27" s="81" t="s">
-        <v>203</v>
-      </c>
-      <c r="J27" s="60" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" thickBot="1">
@@ -3191,28 +3201,28 @@
         <v>27</v>
       </c>
       <c r="B28" s="94" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C28" s="94" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D28" s="94" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E28" s="81">
         <v>2015</v>
       </c>
       <c r="F28" s="94" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G28" s="81">
         <v>6</v>
       </c>
       <c r="H28" s="81" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I28" s="81" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J28" s="83"/>
     </row>
@@ -3221,31 +3231,31 @@
         <v>28</v>
       </c>
       <c r="B29" s="94" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C29" s="94">
         <v>9789568416461</v>
       </c>
       <c r="D29" s="94" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E29" s="81">
         <v>2016</v>
       </c>
       <c r="F29" s="94" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G29" s="81">
         <v>6</v>
       </c>
       <c r="H29" s="81" t="s">
+        <v>208</v>
+      </c>
+      <c r="I29" s="81" t="s">
+        <v>209</v>
+      </c>
+      <c r="J29" s="60" t="s">
         <v>210</v>
-      </c>
-      <c r="I29" s="81" t="s">
-        <v>211</v>
-      </c>
-      <c r="J29" s="60" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" thickBot="1">
@@ -3253,25 +3263,25 @@
         <v>29</v>
       </c>
       <c r="B30" s="94" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C30" s="94">
         <v>9789569853104</v>
       </c>
       <c r="D30" s="94" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E30" s="81">
         <v>2017</v>
       </c>
       <c r="F30" s="94" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G30" s="81">
         <v>6</v>
       </c>
       <c r="H30" s="81" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I30" s="81" t="s">
         <v>108</v>
@@ -3285,26 +3295,26 @@
         <v>30</v>
       </c>
       <c r="B31" s="94" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C31" s="94"/>
       <c r="D31" s="94" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E31" s="81">
         <v>2018</v>
       </c>
       <c r="F31" s="94" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G31" s="81">
         <v>6</v>
       </c>
       <c r="H31" s="81" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I31" s="81" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J31" s="83"/>
     </row>
@@ -3313,31 +3323,31 @@
         <v>31</v>
       </c>
       <c r="B32" s="94" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C32" s="94">
         <v>9786124740831</v>
       </c>
       <c r="D32" s="94" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E32" s="81">
         <v>2018</v>
       </c>
       <c r="F32" s="94" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G32" s="81">
         <v>6</v>
       </c>
       <c r="H32" s="81" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I32" s="81" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J32" s="60" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" thickBot="1">
@@ -3345,7 +3355,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="94" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C33" s="94">
         <v>9786124770265</v>
@@ -3357,16 +3367,16 @@
         <v>2018</v>
       </c>
       <c r="F33" s="94" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G33" s="81">
         <v>6</v>
       </c>
       <c r="H33" s="81" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I33" s="81" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J33" s="84"/>
     </row>
@@ -3375,26 +3385,26 @@
         <v>33</v>
       </c>
       <c r="B34" s="94" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C34" s="96"/>
       <c r="D34" s="96" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E34" s="85">
         <v>2012</v>
       </c>
       <c r="F34" s="96" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G34" s="81">
         <v>6</v>
       </c>
       <c r="H34" s="81" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I34" s="81" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J34" s="82"/>
     </row>
@@ -3586,7 +3596,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="87" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>